<commit_message>
Add auto code generation to excel sheet
</commit_message>
<xml_diff>
--- a/Deviation/RC Model database.xlsx
+++ b/Deviation/RC Model database.xlsx
@@ -9,22 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21180" windowHeight="9675"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21180" windowHeight="9675" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
     <sheet name="Protocols" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Models!$A$1:$G$188</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet2!$A$1:$E$74</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="385">
   <si>
     <t/>
   </si>
@@ -1188,7 +1190,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1204,6 +1206,12 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1234,7 +1242,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1252,6 +1260,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1537,9 +1557,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G188"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1942,10 +1962,10 @@
     </row>
     <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
         <v>15</v>
@@ -1954,10 +1974,10 @@
         <v>16</v>
       </c>
       <c r="E23" t="s">
-        <v>61</v>
-      </c>
-      <c r="G23" t="s">
-        <v>62</v>
+        <v>72</v>
+      </c>
+      <c r="F23" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2176,7 +2196,7 @@
         <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C35" t="s">
         <v>15</v>
@@ -2188,15 +2208,15 @@
         <v>72</v>
       </c>
       <c r="F35" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="B36" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C36" t="s">
         <v>15</v>
@@ -2208,15 +2228,15 @@
         <v>72</v>
       </c>
       <c r="F36" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="C37" t="s">
         <v>15</v>
@@ -2225,10 +2245,10 @@
         <v>16</v>
       </c>
       <c r="E37" t="s">
-        <v>72</v>
-      </c>
-      <c r="F37" t="s">
-        <v>85</v>
+        <v>61</v>
+      </c>
+      <c r="G37" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2776,10 +2796,10 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="B65" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="C65" t="s">
         <v>15</v>
@@ -2788,7 +2808,13 @@
         <v>16</v>
       </c>
       <c r="E65" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="F65" t="s">
+        <v>163</v>
+      </c>
+      <c r="G65" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -2998,10 +3024,10 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="B77" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="C77" t="s">
         <v>15</v>
@@ -3010,13 +3036,7 @@
         <v>16</v>
       </c>
       <c r="E77" t="s">
-        <v>17</v>
-      </c>
-      <c r="F77" t="s">
-        <v>163</v>
-      </c>
-      <c r="G77" t="s">
-        <v>164</v>
+        <v>24</v>
       </c>
     </row>
     <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
@@ -4622,7 +4642,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>249</v>
       </c>
@@ -5171,6 +5191,7 @@
   <autoFilter ref="A1:G188">
     <filterColumn colId="2">
       <filters>
+        <filter val="Hex"/>
         <filter val="Quad"/>
       </filters>
     </filterColumn>
@@ -5181,6 +5202,9 @@
       </filters>
     </filterColumn>
   </autoFilter>
+  <sortState ref="A4:G188">
+    <sortCondition ref="A4"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5190,7 +5214,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5494,4 +5518,2745 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="25" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="130.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="12" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="11" t="str">
+        <f>CHAR(34) &amp; A2 &amp; CHAR(34) &amp; REPT(" ", 15-LEN(A2))</f>
+        <v xml:space="preserve">"Ares"           </v>
+      </c>
+      <c r="G2" s="11" t="str">
+        <f>CHAR(34) &amp; B2 &amp; CHAR(34) &amp; REPT(" ", 20-LEN(B2))</f>
+        <v xml:space="preserve">"Ethos QX75"          </v>
+      </c>
+      <c r="H2" s="11" t="str">
+        <f>"PROTO_NRF24L01_" &amp; UPPER(E2)</f>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I2" s="11" t="str">
+        <f>H2 &amp; REPT(" ", 24-LEN(H2))</f>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J2" s="9" t="str">
+        <f>CONCATENATE("new ModelDBItem(", F2,  ", ", G2, ", buildRFProtoID(TX_NRF24L01, ", I2, ", 0)),")</f>
+        <v>new ModelDBItem("Ares"           , "Ethos QX75"          , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="11" t="str">
+        <f t="shared" ref="F3:F66" si="0">CHAR(34) &amp; A3 &amp; CHAR(34) &amp; REPT(" ", 15-LEN(A3))</f>
+        <v xml:space="preserve">"Attop"          </v>
+      </c>
+      <c r="G3" s="11" t="str">
+        <f t="shared" ref="G3:G66" si="1">CHAR(34) &amp; B3 &amp; CHAR(34) &amp; REPT(" ", 20-LEN(B3))</f>
+        <v xml:space="preserve">"YD717"               </v>
+      </c>
+      <c r="H3" s="11" t="str">
+        <f t="shared" ref="H3:H66" si="2">"PROTO_NRF24L01_" &amp; UPPER(E3)</f>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I3" s="11" t="str">
+        <f t="shared" ref="I3:I66" si="3">H3 &amp; REPT(" ", 24-LEN(H3))</f>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J3" s="9" t="str">
+        <f t="shared" ref="J3:J66" si="4">CONCATENATE("new ModelDBItem(", F3,  ", ", G3, ", buildRFProtoID(TX_NRF24L01, ", I3, ", 0)),")</f>
+        <v>new ModelDBItem("Attop"          , "YD717"               , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Attop"          </v>
+      </c>
+      <c r="G4" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"YD928"               </v>
+      </c>
+      <c r="H4" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I4" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J4" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Attop"          , "YD928"               , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Aviator"        </v>
+      </c>
+      <c r="G5" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"YK016"               </v>
+      </c>
+      <c r="H5" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I5" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J5" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Aviator"        , "YK016"               , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Cheerson"       </v>
+      </c>
+      <c r="G6" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"CX-10"               </v>
+      </c>
+      <c r="H6" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I6" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J6" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Cheerson"       , "CX-10"               , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Cheerson"       </v>
+      </c>
+      <c r="G7" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"CX-11"               </v>
+      </c>
+      <c r="H7" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I7" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J7" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Cheerson"       , "CX-11"               , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Cheerson"       </v>
+      </c>
+      <c r="G8" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"CX-205/SH6057"       </v>
+      </c>
+      <c r="H8" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I8" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J8" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Cheerson"       , "CX-205/SH6057"       , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Cheerson"       </v>
+      </c>
+      <c r="G9" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"CX-30"               </v>
+      </c>
+      <c r="H9" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I9" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J9" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Cheerson"       , "CX-30"               , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"CrazyFlie"      </v>
+      </c>
+      <c r="G10" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"Nano"                </v>
+      </c>
+      <c r="H10" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_CFLIE</v>
+      </c>
+      <c r="I10" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_CFLIE    </v>
+      </c>
+      <c r="J10" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("CrazyFlie"      , "Nano"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_CFLIE    , 0)),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Flytecs"        </v>
+      </c>
+      <c r="G11" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"X-Drone Nano"        </v>
+      </c>
+      <c r="H11" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I11" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J11" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Flytecs"        , "X-Drone Nano"        , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Hisky"          </v>
+      </c>
+      <c r="G12" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"FF120"               </v>
+      </c>
+      <c r="H12" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_HISKY</v>
+      </c>
+      <c r="I12" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_HISKY    </v>
+      </c>
+      <c r="J12" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Hisky"          , "FF120"               , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_HISKY    , 0)),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Hisky"          </v>
+      </c>
+      <c r="G13" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"HMX120"              </v>
+      </c>
+      <c r="H13" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_HISKY</v>
+      </c>
+      <c r="I13" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_HISKY    </v>
+      </c>
+      <c r="J13" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Hisky"          , "HMX120"              , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_HISKY    , 0)),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"HobbyKing"      </v>
+      </c>
+      <c r="G14" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"Q-Bot Micro"         </v>
+      </c>
+      <c r="H14" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_HISKY</v>
+      </c>
+      <c r="I14" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_HISKY    </v>
+      </c>
+      <c r="J14" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("HobbyKing"      , "Q-Bot Micro"         , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_HISKY    , 0)),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Huan"           </v>
+      </c>
+      <c r="G15" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"QI 881"              </v>
+      </c>
+      <c r="H15" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_SYMAX</v>
+      </c>
+      <c r="I15" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_SYMAX    </v>
+      </c>
+      <c r="J15" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Huan"           , "QI 881"              , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_SYMAX    , 0)),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Huaxiang Toys"  </v>
+      </c>
+      <c r="G16" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"Sky Walker 8983"     </v>
+      </c>
+      <c r="H16" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I16" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J16" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Huaxiang Toys"  , "Sky Walker 8983"     , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"JD"             </v>
+      </c>
+      <c r="G17" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"JXD 385"             </v>
+      </c>
+      <c r="H17" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I17" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J17" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("JD"             , "JXD 385"             , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"JD"             </v>
+      </c>
+      <c r="G18" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"JXD 388"             </v>
+      </c>
+      <c r="H18" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I18" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J18" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("JD"             , "JXD 388"             , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"JD"             </v>
+      </c>
+      <c r="G19" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"JXD 389"             </v>
+      </c>
+      <c r="H19" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I19" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J19" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("JD"             , "JXD 389"             , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"JD"             </v>
+      </c>
+      <c r="G20" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"JXD 390"             </v>
+      </c>
+      <c r="H20" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I20" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J20" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("JD"             , "JXD 390"             , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"JD"             </v>
+      </c>
+      <c r="G21" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"JXD 391"             </v>
+      </c>
+      <c r="H21" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I21" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J21" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("JD"             , "JXD 391"             , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"JD"             </v>
+      </c>
+      <c r="G22" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"JXD 392"             </v>
+      </c>
+      <c r="H22" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I22" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J22" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("JD"             , "JXD 392"             , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"JD"             </v>
+      </c>
+      <c r="G23" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"JXD 393"             </v>
+      </c>
+      <c r="H23" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I23" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J23" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("JD"             , "JXD 393"             , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"JIAYUAN"        </v>
+      </c>
+      <c r="G24" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"S-2"                 </v>
+      </c>
+      <c r="H24" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I24" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J24" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("JIAYUAN"        , "S-2"                 , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"JJR/C"          </v>
+      </c>
+      <c r="G25" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"1000A"               </v>
+      </c>
+      <c r="H25" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I25" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J25" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("JJR/C"          , "1000A"               , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"JJR/C"          </v>
+      </c>
+      <c r="G26" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"F180"                </v>
+      </c>
+      <c r="H26" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I26" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J26" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("JJR/C"          , "F180"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"JJR/C"          </v>
+      </c>
+      <c r="G27" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"F182"                </v>
+      </c>
+      <c r="H27" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I27" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J27" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("JJR/C"          , "F182"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"JJR/C"          </v>
+      </c>
+      <c r="G28" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"H8C"                 </v>
+      </c>
+      <c r="H28" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I28" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J28" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("JJR/C"          , "H8C"                 , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Landbow"        </v>
+      </c>
+      <c r="G29" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"X-Dart Next"         </v>
+      </c>
+      <c r="H29" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I29" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J29" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Landbow"        , "X-Dart Next"         , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Ni Hui"         </v>
+      </c>
+      <c r="G30" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"U207"                </v>
+      </c>
+      <c r="H30" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I30" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J30" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Ni Hui"         , "U207"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Nincoair"       </v>
+      </c>
+      <c r="G31" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"Quadrone"            </v>
+      </c>
+      <c r="H31" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I31" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J31" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Nincoair"       , "Quadrone"            , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A32" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Sanlianhuan"    </v>
+      </c>
+      <c r="G32" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"SH 6043 Ladybug"     </v>
+      </c>
+      <c r="H32" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I32" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J32" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Sanlianhuan"    , "SH 6043 Ladybug"     , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Sanlianhuan"    </v>
+      </c>
+      <c r="G33" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"SH 6044"             </v>
+      </c>
+      <c r="H33" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I33" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J33" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Sanlianhuan"    , "SH 6044"             , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Sanlianhuan"    </v>
+      </c>
+      <c r="G34" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"SH 6046 Puffer"      </v>
+      </c>
+      <c r="H34" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I34" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J34" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Sanlianhuan"    , "SH 6046 Puffer"      , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Sanlianhuan"    </v>
+      </c>
+      <c r="G35" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"SH 6048 F22"         </v>
+      </c>
+      <c r="H35" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I35" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J35" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Sanlianhuan"    , "SH 6048 F22"         , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Sky Walker"     </v>
+      </c>
+      <c r="G36" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"HM-1306"             </v>
+      </c>
+      <c r="H36" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I36" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J36" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Sky Walker"     , "HM-1306"             , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Skybotz"        </v>
+      </c>
+      <c r="G37" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"Mini UFO"            </v>
+      </c>
+      <c r="H37" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I37" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J37" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Skybotz"        , "Mini UFO"            , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Skyline"        </v>
+      </c>
+      <c r="G38" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"YD717"               </v>
+      </c>
+      <c r="H38" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I38" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J38" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Skyline"        , "YD717"               , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F39" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Syma"           </v>
+      </c>
+      <c r="G39" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"X2"                  </v>
+      </c>
+      <c r="H39" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_SYMAX</v>
+      </c>
+      <c r="I39" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_SYMAX    </v>
+      </c>
+      <c r="J39" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Syma"           , "X2"                  , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_SYMAX    , 0)),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Syma"           </v>
+      </c>
+      <c r="G40" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"X3"                  </v>
+      </c>
+      <c r="H40" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I40" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J40" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Syma"           , "X3"                  , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F41" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Syma"           </v>
+      </c>
+      <c r="G41" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"X4"                  </v>
+      </c>
+      <c r="H41" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I41" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J41" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Syma"           , "X4"                  , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Syma"           </v>
+      </c>
+      <c r="G42" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"X5C"                 </v>
+      </c>
+      <c r="H42" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_SYMAX</v>
+      </c>
+      <c r="I42" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_SYMAX    </v>
+      </c>
+      <c r="J42" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Syma"           , "X5C"                 , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_SYMAX    , 0)),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F43" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Syma"           </v>
+      </c>
+      <c r="G43" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"X5C-1"               </v>
+      </c>
+      <c r="H43" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_SYMAX</v>
+      </c>
+      <c r="I43" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_SYMAX    </v>
+      </c>
+      <c r="J43" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Syma"           , "X5C-1"               , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_SYMAX    , 0)),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Syma"           </v>
+      </c>
+      <c r="G44" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"X6"                  </v>
+      </c>
+      <c r="H44" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I44" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J44" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Syma"           , "X6"                  , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F45" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Syma"           </v>
+      </c>
+      <c r="G45" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"X7"                  </v>
+      </c>
+      <c r="H45" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_SYMAX</v>
+      </c>
+      <c r="I45" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_SYMAX    </v>
+      </c>
+      <c r="J45" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Syma"           , "X7"                  , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_SYMAX    , 0)),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F46" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Syma"           </v>
+      </c>
+      <c r="G46" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"X8C"                 </v>
+      </c>
+      <c r="H46" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_SYMAX</v>
+      </c>
+      <c r="I46" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_SYMAX    </v>
+      </c>
+      <c r="J46" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Syma"           , "X8C"                 , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_SYMAX    , 0)),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F47" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Syma"           </v>
+      </c>
+      <c r="G47" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"X11"                 </v>
+      </c>
+      <c r="H47" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_SYMAX</v>
+      </c>
+      <c r="I47" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_SYMAX    </v>
+      </c>
+      <c r="J47" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Syma"           , "X11"                 , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_SYMAX    , 0)),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F48" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Syma"           </v>
+      </c>
+      <c r="G48" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"X12"                 </v>
+      </c>
+      <c r="H48" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_SYMAX</v>
+      </c>
+      <c r="I48" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_SYMAX    </v>
+      </c>
+      <c r="J48" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Syma"           , "X12"                 , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_SYMAX    , 0)),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Toybase"        </v>
+      </c>
+      <c r="G49" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"L6036"               </v>
+      </c>
+      <c r="H49" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I49" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J49" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Toybase"        , "L6036"               , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"Toybase"        </v>
+      </c>
+      <c r="G50" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"L6038"               </v>
+      </c>
+      <c r="H50" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I50" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J50" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("Toybase"        , "L6038"               , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F51" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"WL TOYS"        </v>
+      </c>
+      <c r="G51" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"v202"                </v>
+      </c>
+      <c r="H51" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I51" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J51" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("WL TOYS"        , "v202"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F52" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"WL TOYS"        </v>
+      </c>
+      <c r="G52" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"v212"                </v>
+      </c>
+      <c r="H52" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I52" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J52" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("WL TOYS"        , "v212"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F53" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"WL TOYS"        </v>
+      </c>
+      <c r="G53" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"v222"                </v>
+      </c>
+      <c r="H53" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I53" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J53" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("WL TOYS"        , "v222"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F54" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"WL TOYS"        </v>
+      </c>
+      <c r="G54" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"v252"                </v>
+      </c>
+      <c r="H54" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I54" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J54" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("WL TOYS"        , "v252"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F55" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"WL TOYS"        </v>
+      </c>
+      <c r="G55" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"v252 Pro"            </v>
+      </c>
+      <c r="H55" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I55" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J55" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("WL TOYS"        , "v252 Pro"            , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F56" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"WL TOYS"        </v>
+      </c>
+      <c r="G56" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"v262"                </v>
+      </c>
+      <c r="H56" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I56" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J56" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("WL TOYS"        , "v262"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F57" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"WL TOYS"        </v>
+      </c>
+      <c r="G57" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"v272"                </v>
+      </c>
+      <c r="H57" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I57" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J57" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("WL TOYS"        , "v272"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="E58" s="10"/>
+      <c r="F58" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"WL TOYS"        </v>
+      </c>
+      <c r="G58" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"v282"                </v>
+      </c>
+      <c r="H58" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_</v>
+      </c>
+      <c r="I58" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_         </v>
+      </c>
+      <c r="J58" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("WL TOYS"        , "v282"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_         , 0)),</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="E59" s="10"/>
+      <c r="F59" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"WL TOYS"        </v>
+      </c>
+      <c r="G59" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"v292"                </v>
+      </c>
+      <c r="H59" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_</v>
+      </c>
+      <c r="I59" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_         </v>
+      </c>
+      <c r="J59" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("WL TOYS"        , "v292"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_         , 0)),</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F60" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"WL TOYS"        </v>
+      </c>
+      <c r="G60" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"v323"                </v>
+      </c>
+      <c r="H60" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I60" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J60" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("WL TOYS"        , "v323"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F61" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"WL TOYS"        </v>
+      </c>
+      <c r="G61" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"v333"                </v>
+      </c>
+      <c r="H61" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I61" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J61" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("WL TOYS"        , "v333"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F62" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"WL TOYS"        </v>
+      </c>
+      <c r="G62" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"v343"                </v>
+      </c>
+      <c r="H62" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I62" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J62" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("WL TOYS"        , "v343"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F63" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"WL TOYS"        </v>
+      </c>
+      <c r="G63" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"v353"                </v>
+      </c>
+      <c r="H63" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I63" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J63" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("WL TOYS"        , "v353"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F64" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"WL TOYS"        </v>
+      </c>
+      <c r="G64" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"v393"                </v>
+      </c>
+      <c r="H64" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I64" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J64" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("WL TOYS"        , "v393"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F65" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"WL TOYS"        </v>
+      </c>
+      <c r="G65" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"v626"                </v>
+      </c>
+      <c r="H65" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I65" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J65" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("WL TOYS"        , "v626"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F66" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">"WL TOYS"        </v>
+      </c>
+      <c r="G66" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">"v636"                </v>
+      </c>
+      <c r="H66" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I66" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J66" s="9" t="str">
+        <f t="shared" si="4"/>
+        <v>new ModelDBItem("WL TOYS"        , "v636"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F67" s="11" t="str">
+        <f t="shared" ref="F67:F74" si="5">CHAR(34) &amp; A67 &amp; CHAR(34) &amp; REPT(" ", 15-LEN(A67))</f>
+        <v xml:space="preserve">"WL TOYS"        </v>
+      </c>
+      <c r="G67" s="11" t="str">
+        <f t="shared" ref="G67:G74" si="6">CHAR(34) &amp; B67 &amp; CHAR(34) &amp; REPT(" ", 20-LEN(B67))</f>
+        <v xml:space="preserve">"v666"                </v>
+      </c>
+      <c r="H67" s="11" t="str">
+        <f t="shared" ref="H67:H74" si="7">"PROTO_NRF24L01_" &amp; UPPER(E67)</f>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I67" s="11" t="str">
+        <f t="shared" ref="I67:I74" si="8">H67 &amp; REPT(" ", 24-LEN(H67))</f>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J67" s="9" t="str">
+        <f t="shared" ref="J67:J74" si="9">CONCATENATE("new ModelDBItem(", F67,  ", ", G67, ", buildRFProtoID(TX_NRF24L01, ", I67, ", 0)),")</f>
+        <v>new ModelDBItem("WL TOYS"        , "v666"                , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F68" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"XINXUN"         </v>
+      </c>
+      <c r="G68" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"X28"                 </v>
+      </c>
+      <c r="H68" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I68" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J68" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v>new ModelDBItem("XINXUN"         , "X28"                 , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F69" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"XINXUN"         </v>
+      </c>
+      <c r="G69" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"X30"                 </v>
+      </c>
+      <c r="H69" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I69" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J69" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v>new ModelDBItem("XINXUN"         , "X30"                 , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F70" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"XINXUN"         </v>
+      </c>
+      <c r="G70" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"X33"                 </v>
+      </c>
+      <c r="H70" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I70" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J70" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v>new ModelDBItem("XINXUN"         , "X33"                 , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>353</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F71" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"XINXUN"         </v>
+      </c>
+      <c r="G71" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"X39"                 </v>
+      </c>
+      <c r="H71" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I71" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J71" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v>new ModelDBItem("XINXUN"         , "X39"                 , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F72" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"XINXUN"         </v>
+      </c>
+      <c r="G72" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"X40"                 </v>
+      </c>
+      <c r="H72" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>PROTO_NRF24L01_YD717</v>
+      </c>
+      <c r="I72" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PROTO_NRF24L01_YD717    </v>
+      </c>
+      <c r="J72" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v>new ModelDBItem("XINXUN"         , "X40"                 , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F73" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"YI ZHAN"        </v>
+      </c>
+      <c r="G73" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"X4"                  </v>
+      </c>
+      <c r="H73" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I73" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J73" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v>new ModelDBItem("YI ZHAN"        , "X4"                  , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D74" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F74" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">"YI ZHAN"        </v>
+      </c>
+      <c r="G74" s="11" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">"X6"                  </v>
+      </c>
+      <c r="H74" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v>PROTO_NRF24L01_V2X2</v>
+      </c>
+      <c r="I74" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">PROTO_NRF24L01_V2X2     </v>
+      </c>
+      <c r="J74" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v>new ModelDBItem("YI ZHAN"        , "X6"                  , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E74"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Codes are branched to UniConTX
</commit_message>
<xml_diff>
--- a/Deviation/RC Model database.xlsx
+++ b/Deviation/RC Model database.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\17.Deviation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\07.Schematic\Schematics\Deviation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21180" windowHeight="9675" activeTab="3"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21180" windowHeight="9675" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
     <sheet name="Protocols" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Models!$A$1:$G$188</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1847" uniqueCount="386">
   <si>
     <t/>
   </si>
@@ -1181,6 +1182,9 @@
   </si>
   <si>
     <t>NRF24L01 Set</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
   </si>
 </sst>
 </file>
@@ -1190,7 +1194,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1213,6 +1217,13 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1228,12 +1239,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1242,7 +1268,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1271,6 +1297,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1559,7 +1594,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:E1"/>
+      <selection pane="bottomLeft" sqref="A1:D188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2251,7 +2286,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -2351,7 +2386,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>89</v>
       </c>
@@ -2371,7 +2406,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>89</v>
       </c>
@@ -2391,7 +2426,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>89</v>
       </c>
@@ -2411,7 +2446,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>89</v>
       </c>
@@ -3289,7 +3324,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>190</v>
       </c>
@@ -3556,7 +3591,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>212</v>
       </c>
@@ -3573,7 +3608,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>212</v>
       </c>
@@ -3675,7 +3710,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>212</v>
       </c>
@@ -4204,7 +4239,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>249</v>
       </c>
@@ -4287,7 +4322,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>249</v>
       </c>
@@ -4327,7 +4362,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>249</v>
       </c>
@@ -4367,7 +4402,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>249</v>
       </c>
@@ -4602,7 +4637,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>249</v>
       </c>
@@ -4622,7 +4657,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>249</v>
       </c>
@@ -4800,7 +4835,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>249</v>
       </c>
@@ -4843,7 +4878,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>249</v>
       </c>
@@ -5197,8 +5232,9 @@
     </filterColumn>
     <filterColumn colId="3">
       <filters>
+        <filter val="A7105"/>
+        <filter val="CYRF6936"/>
         <filter val="NRF24L01"/>
-        <filter val="NRF24L01 ?"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -5524,7 +5560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
@@ -5853,7 +5889,7 @@
         <v>new ModelDBItem("Cheerson"       , "CX-30"               , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>48</v>
       </c>
@@ -6001,7 +6037,7 @@
         <v>new ModelDBItem("Hisky"          , "HMX120"              , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_HISKY    , 0)),</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>87</v>
       </c>
@@ -6667,7 +6703,7 @@
         <v>new ModelDBItem("Nincoair"       , "Quadrone"            , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_V2X2     , 0)),</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
         <v>168</v>
       </c>
@@ -6704,7 +6740,7 @@
         <v>new ModelDBItem("Sanlianhuan"    , "SH 6043 Ladybug"     , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>168</v>
       </c>
@@ -6741,7 +6777,7 @@
         <v>new ModelDBItem("Sanlianhuan"    , "SH 6044"             , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
         <v>168</v>
       </c>
@@ -6778,7 +6814,7 @@
         <v>new ModelDBItem("Sanlianhuan"    , "SH 6046 Puffer"      , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>168</v>
       </c>
@@ -6815,7 +6851,7 @@
         <v>new ModelDBItem("Sanlianhuan"    , "SH 6048 F22"         , buildRFProtoID(TX_NRF24L01, PROTO_NRF24L01_YD717    , 0)),</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="24" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
         <v>176</v>
       </c>
@@ -8259,4 +8295,1230 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D86"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D86"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>385</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>322</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D74" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="C79" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="B80" s="14" t="s">
+        <v>348</v>
+      </c>
+      <c r="C80" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="B81" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="B84" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="B85" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="B86" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>